<commit_message>
Update R and Datasets
</commit_message>
<xml_diff>
--- a/R Scripts/Dataset/CRQ2_1.xlsx
+++ b/R Scripts/Dataset/CRQ2_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edusm\OneDrive\Documentos\uff\dissertacao\git\feature-toggles\R Scripts\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_C556DD5B346193E508318B83E2DC1529B9D687EF" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4B036F8A-C601-4D6A-BF00-BD9D678D4C29}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_C556DD5B346193E508318B83E2DC1529B9D687EF" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8B144343-6EEB-458B-8A64-A8DAF940EAEB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="3255" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,10 @@
     <t>id</t>
   </si>
   <si>
-    <t>NUM_MERGES_100 COMMITS_SEM_FW</t>
+    <t>NUM_MERGES_PER_100_COMMITS_WO_FT</t>
   </si>
   <si>
-    <t>NUM_MERGES_100 COMMITS_COM_FW</t>
+    <t>NUM_MERGES_PER_100_COMMITS_WITH_FT</t>
   </si>
 </sst>
 </file>
@@ -378,12 +378,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adds new scripts for the analyses by language
</commit_message>
<xml_diff>
--- a/R Scripts/Dataset/CRQ2_1.xlsx
+++ b/R Scripts/Dataset/CRQ2_1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edusm\OneDrive\Documentos\uff\dissertacao\git\feature-toggles\R Scripts\Dataset\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_C556DD5B346193E508318B83E2DC1529B9D687EF" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8B144343-6EEB-458B-8A64-A8DAF940EAEB}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="3255" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="3255" windowWidth="15375" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -35,11 +29,32 @@
   <si>
     <t>NUM_MERGES_PER_100_COMMITS_WITH_FT</t>
   </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>c#</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Linguagem</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,7 +206,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,1772 +383,2249 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C159"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>347655</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>4.634971155758902</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>9.3489988113742335</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>489645</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>4.314868804664723</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>5.3617699820609923</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>552695</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>2.3529411764705883</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>769182</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>7.9234972677595632</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>806511</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>29.83606557377049</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>15.716272600834492</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1059929</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
         <v>8.8573959255978746E-2</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.82256169212690955</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1217077</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>29.907379743053482</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>16.329704510108865</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1338040</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>16.033971144991302</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>18.06640625</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1352520</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
         <v>6.1296859169199598</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>22.405838436372786</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1722606</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
         <v>13.399857448325017</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>19.617224880382775</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1799884</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
         <v>16.016427104722794</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>22.044917257683217</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1848736</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
         <v>2.2408963585434174</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2.512562814070352</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2263742</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
         <v>15.177971793149766</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>19.14936914936915</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2386842</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
         <v>29.889519259480441</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>16.560509554140129</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2392358</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
         <v>7.7205882352941178</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>1.0869565217391304</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2416064</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
         <v>9.0609942413914677</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>16.449109190333392</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2577146</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.43196544276457882</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2723436</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
         <v>7.4003795066413662</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>9.0707262924199181</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2987495</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
         <v>4.3003109729009328</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>2.402745995423341</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2995765</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>3.3393501805054151</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4494078</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
         <v>2.6785714285714284</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>1.4184397163120568</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4693087</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
         <v>10.515916575192097</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>2.8209321340964841</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5021616</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
         <v>29.952124476361462</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>15.760111576011157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5144181</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
         <v>4.4544867656552611</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>6.2827225130890056</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5197539</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
         <v>3.4270650263620386</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>7.3033707865168536</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5203368</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
         <v>2.43161094224924</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>1.2847965738758029</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5287954</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
         <v>29.83606557377049</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>16.005665722379604</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5421677</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
         <v>22.568093385214009</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>13.846153846153847</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5541660</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
         <v>6.6511085180863478</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>9.183673469387756</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5614312</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>1.0695187165775402</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6127047</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
         <v>12.726008344923505</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6388572</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
         <v>4.026845637583893</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>19.458128078817733</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7031510</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
         <v>7.773722627737226</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7358191</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
         <v>11.149825783972126</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>1.7094017094017093</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8484604</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36">
         <v>7.9602305110505984</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8884773</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
         <v>11.409395973154362</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>8.2444918265813794</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10199599</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38">
         <v>25.401942217028651</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>26.60217654171705</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10391073</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39">
         <v>18.044468154019089</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>26.408304498269896</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10934610</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
         <v>9.420289855072463</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>11.46384479717813</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>11246402</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41">
         <v>2.0588235294117645</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>1.1976047904191616</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11671912</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42">
         <v>4.1131105398457581</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>3.5343035343035343</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12736575</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
         <v>0</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>22.750139742873113</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13633443</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
         <v>17.107750472589792</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>14.117647058823529</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>15008139</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45">
         <v>5.2287581699346406</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>1.3303769401330376</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15344614</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46">
         <v>1.6994633273703041</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>3.9370078740157481</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>16416867</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
         <v>4.5951859956236323</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>10.936961763692732</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>16619668</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48">
         <v>0</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>1.1754068716094033</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>16827151</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
         <v>2.3178807947019866</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>13.354632587859426</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>17164513</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50">
         <v>12.400455062571103</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>18355156</v>
       </c>
-      <c r="B51">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51">
         <v>1.5544041450777202</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>18625008</v>
       </c>
-      <c r="B52">
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52">
         <v>0.93896713615023475</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>1.8404907975460123</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>18810181</v>
       </c>
-      <c r="B53">
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
         <v>0.89686098654708524</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>19272646</v>
       </c>
-      <c r="B54">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
         <v>8.4991708126036478</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>2.2787028921998247</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19695722</v>
       </c>
-      <c r="B55">
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55">
         <v>17.387616624257845</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>14.41753171856978</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20538228</v>
       </c>
-      <c r="B56">
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56">
         <v>7.3878627968337733</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>22.299336149668076</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>20767408</v>
       </c>
-      <c r="B57">
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57">
         <v>16.101694915254239</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>15.730337078651685</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>21674470</v>
       </c>
-      <c r="B58">
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58">
         <v>0.80645161290322576</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>22128680</v>
       </c>
-      <c r="B59">
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59">
         <v>11.307420494699647</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>17.21311475409836</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>23700996</v>
       </c>
-      <c r="B60">
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60">
         <v>0.38860103626943004</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>23722245</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61">
         <v>0.53908355795148244</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>23996209</v>
       </c>
-      <c r="B62">
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62">
         <v>0.2386634844868735</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>24676571</v>
       </c>
-      <c r="B63">
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63">
         <v>6.6838046272493576</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>12.693498452012383</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>24728203</v>
       </c>
-      <c r="B64">
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64">
         <v>4.5472363778910232</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>7.0355441553682665</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>24850244</v>
       </c>
-      <c r="B65">
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65">
         <v>22.393822393822393</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>15.859030837004406</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>24998407</v>
       </c>
-      <c r="B66">
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66">
         <v>24.043179587831208</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>30.764029749830968</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>25745061</v>
       </c>
-      <c r="B67">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
         <v>10.636900853578464</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>26113177</v>
       </c>
-      <c r="B68">
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68">
         <v>15.254237288135593</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>14.166666666666666</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>26767408</v>
       </c>
-      <c r="B69">
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69">
         <v>30.944444444444443</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>28.381962864721487</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>27058591</v>
       </c>
-      <c r="B70">
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70">
         <v>4.314868804664723</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>0.57686760888376121</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>27288669</v>
       </c>
-      <c r="B71">
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71">
         <v>0</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>1.0416666666666667</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28054380</v>
       </c>
-      <c r="B72">
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72">
         <v>16.22983870967742</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>24.382207578253706</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>29340261</v>
       </c>
-      <c r="B73">
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73">
         <v>14.100486223662886</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>29364795</v>
       </c>
-      <c r="B74">
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74">
         <v>4.314868804664723</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>0.42504958911873053</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>29641957</v>
       </c>
-      <c r="B75">
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75">
         <v>0</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>1.1111111111111112</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>30175039</v>
       </c>
-      <c r="B76">
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76">
         <v>13.636363636363637</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>4.2105263157894735</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>30702818</v>
       </c>
-      <c r="B77">
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77">
         <v>0</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>1.1135857461024499</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>31377627</v>
       </c>
-      <c r="B78">
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78">
         <v>8.5738184859891255</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>2.3235031277926721</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>32340528</v>
       </c>
-      <c r="B79">
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79">
         <v>8.5526315789473681</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <v>13.274336283185841</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>34396268</v>
       </c>
-      <c r="B80">
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80">
         <v>9.8591549295774641</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>3.2590051457975986</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>35300278</v>
       </c>
-      <c r="B81">
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81">
         <v>30.952380952380953</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>28.877005347593585</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>35489525</v>
       </c>
-      <c r="B82">
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82">
         <v>11.022997620935765</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>11.956521739130435</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>39788762</v>
       </c>
-      <c r="B83">
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83">
         <v>27.737226277372262</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>28.972972972972972</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>41607639</v>
       </c>
-      <c r="B84">
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84">
         <v>1.502145922746781</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>42480983</v>
       </c>
-      <c r="B85">
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85">
         <v>0.23148148148148148</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>0.42704626334519574</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>42585709</v>
       </c>
-      <c r="B86">
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86">
         <v>4.3795620437956204</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>1.5789473684210527</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>42682761</v>
       </c>
-      <c r="B87">
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87">
         <v>27.411167512690355</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <v>28.225806451612904</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>45260412</v>
       </c>
-      <c r="B88">
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88">
         <v>13.436692506459949</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <v>12.320916905444125</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>45866355</v>
       </c>
-      <c r="B89">
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89">
         <v>0.73126142595978061</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>45931203</v>
       </c>
-      <c r="B90">
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90">
         <v>4.314868804664723</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>4.1289467873702801</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>47632133</v>
       </c>
-      <c r="B91">
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91">
         <v>15.19047619047619</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <v>9.6947935368043083</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>49892996</v>
       </c>
-      <c r="B92">
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92">
         <v>6.2706270627062706</v>
       </c>
-      <c r="C92">
+      <c r="D92">
         <v>7.2796934865900385</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>50365703</v>
       </c>
-      <c r="B93">
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93">
         <v>26.65036674816626</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>26.522593320235757</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>50667950</v>
       </c>
-      <c r="B94">
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94">
         <v>26.632653061224488</v>
       </c>
-      <c r="C94">
+      <c r="D94">
         <v>17.543859649122808</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>51774067</v>
       </c>
-      <c r="B95">
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95">
         <v>0.96153846153846156</v>
       </c>
-      <c r="C95">
+      <c r="D95">
         <v>3.6764705882352939</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>53135203</v>
       </c>
-      <c r="B96">
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96">
         <v>2.6338893766461808</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>3.3240997229916895</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>53534987</v>
       </c>
-      <c r="B97">
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97">
         <v>4.8</v>
       </c>
-      <c r="C97">
+      <c r="D97">
         <v>2.8846153846153846</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>54648215</v>
       </c>
-      <c r="B98">
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98">
         <v>21.47627416520211</v>
       </c>
-      <c r="C98">
+      <c r="D98">
         <v>28.093492208982585</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>62129589</v>
       </c>
-      <c r="B99">
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99">
         <v>0.79365079365079361</v>
       </c>
-      <c r="C99">
+      <c r="D99">
         <v>1.7605633802816902</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>68407220</v>
       </c>
-      <c r="B100">
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100">
         <v>1.5107212475633529</v>
       </c>
-      <c r="C100">
+      <c r="D100">
         <v>3.4954407294832825</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>68464903</v>
       </c>
-      <c r="B101">
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101">
         <v>16.033971144991302</v>
       </c>
-      <c r="C101">
+      <c r="D101">
         <v>21.34107027724049</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>69359362</v>
       </c>
-      <c r="B102">
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102">
         <v>8.9348813730439165</v>
       </c>
-      <c r="C102">
+      <c r="D102">
         <v>8.5020242914979764</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>71187431</v>
       </c>
-      <c r="B103">
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103">
         <v>1.1494252873563218</v>
       </c>
-      <c r="C103">
+      <c r="D103">
         <v>14.720812182741117</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>71376869</v>
       </c>
-      <c r="B104">
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104">
         <v>9.387755102040817</v>
       </c>
-      <c r="C104">
+      <c r="D104">
         <v>9.4117647058823533</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>71501855</v>
       </c>
-      <c r="B105">
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105">
         <v>0.6211180124223602</v>
       </c>
-      <c r="C105">
+      <c r="D105">
         <v>9.7742363877822047</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>72233269</v>
       </c>
-      <c r="B106">
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
         <v>12.681912681912682</v>
       </c>
-      <c r="C106">
+      <c r="D106">
         <v>8.870967741935484</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>72479761</v>
       </c>
-      <c r="B107">
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107">
         <v>6.1764705882352944</v>
       </c>
-      <c r="C107">
+      <c r="D107">
         <v>4.1193778898696936</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>73205358</v>
       </c>
-      <c r="B108">
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108">
         <v>17.248062015503876</v>
       </c>
-      <c r="C108">
+      <c r="D108">
         <v>21.025328043942629</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>73714491</v>
       </c>
-      <c r="B109">
+      <c r="B109" t="s">
+        <v>3</v>
+      </c>
+      <c r="C109">
         <v>13.939393939393939</v>
       </c>
-      <c r="C109">
+      <c r="D109">
         <v>5.9285714285714288</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>74074978</v>
       </c>
-      <c r="B110">
+      <c r="B110" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110">
         <v>13.939393939393939</v>
       </c>
-      <c r="C110">
+      <c r="D110">
         <v>5.3231939163498101</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>74275100</v>
       </c>
-      <c r="B111">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111">
         <v>0</v>
       </c>
-      <c r="C111">
+      <c r="D111">
         <v>1.1764705882352942</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>75758799</v>
       </c>
-      <c r="B112">
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112">
         <v>10.95890410958904</v>
       </c>
-      <c r="C112">
+      <c r="D112">
         <v>7.0264765784114056</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>76819000</v>
       </c>
-      <c r="B113">
+      <c r="B113" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113">
         <v>4.314868804664723</v>
       </c>
-      <c r="C113">
+      <c r="D113">
         <v>5.3759094583670173</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>78471377</v>
       </c>
-      <c r="B114">
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114">
         <v>0.90909090909090906</v>
       </c>
-      <c r="C114">
+      <c r="D114">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>79148749</v>
       </c>
-      <c r="B115">
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115">
         <v>4.8458149779735686</v>
       </c>
-      <c r="C115">
+      <c r="D115">
         <v>6.25</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>79465598</v>
       </c>
-      <c r="B116">
+      <c r="B116" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116">
         <v>21.851851851851851</v>
       </c>
-      <c r="C116">
+      <c r="D116">
         <v>30.145278450363197</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>84507987</v>
       </c>
-      <c r="B117">
+      <c r="B117" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117">
         <v>23.79032258064516</v>
       </c>
-      <c r="C117">
+      <c r="D117">
         <v>33.2409972299169</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>86124349</v>
       </c>
-      <c r="B118">
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118">
         <v>23.79032258064516</v>
       </c>
-      <c r="C118">
+      <c r="D118">
         <v>33.111702127659576</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>86282367</v>
       </c>
-      <c r="B119">
+      <c r="B119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119">
         <v>17.559681697612731</v>
       </c>
-      <c r="C119">
+      <c r="D119">
         <v>5.913978494623656</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>89386914</v>
       </c>
-      <c r="B120">
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120">
         <v>13.313046785850133</v>
       </c>
-      <c r="C120">
+      <c r="D120">
         <v>15.570419918246005</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>92938357</v>
       </c>
-      <c r="B121">
+      <c r="B121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121">
         <v>13.315579227696405</v>
       </c>
-      <c r="C121">
+      <c r="D121">
         <v>7.4074074074074074</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>93316749</v>
       </c>
-      <c r="B122">
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
         <v>2.2013596633214632</v>
       </c>
-      <c r="C122">
+      <c r="D122">
         <v>0.56603773584905659</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>93964532</v>
       </c>
-      <c r="B123">
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123">
         <v>3.0895983522142121</v>
       </c>
-      <c r="C123">
+      <c r="D123">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>94167681</v>
       </c>
-      <c r="B124">
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124">
         <v>13.315579227696405</v>
       </c>
-      <c r="C124">
+      <c r="D124">
         <v>9.2879256965944279</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>95210715</v>
       </c>
-      <c r="B125">
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125">
         <v>13.296556971656839</v>
       </c>
-      <c r="C125">
+      <c r="D125">
         <v>9.0909090909090917</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>95443579</v>
       </c>
-      <c r="B126">
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126">
         <v>13.296556971656839</v>
       </c>
-      <c r="C126">
+      <c r="D126">
         <v>9.2731829573934839</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>96212237</v>
       </c>
-      <c r="B127">
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127">
         <v>24.230783302235395</v>
       </c>
-      <c r="C127">
+      <c r="D127">
         <v>24.817993489197988</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>96530667</v>
       </c>
-      <c r="B128">
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128">
         <v>20.047827819848546</v>
       </c>
-      <c r="C128">
+      <c r="D128">
         <v>6.1797752808988768</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>97128753</v>
       </c>
-      <c r="B129">
+      <c r="B129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129">
         <v>31.976459048553213</v>
       </c>
-      <c r="C129">
+      <c r="D129">
         <v>20.987654320987655</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>98375316</v>
       </c>
-      <c r="B130">
+      <c r="B130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130">
         <v>23.94243022413233</v>
       </c>
-      <c r="C130">
+      <c r="D130">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>98575487</v>
       </c>
-      <c r="B131">
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131">
         <v>20.613713743912424</v>
       </c>
-      <c r="C131">
+      <c r="D131">
         <v>28.357142857142858</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>101262862</v>
       </c>
-      <c r="B132">
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132">
         <v>13.282588011417698</v>
       </c>
-      <c r="C132">
+      <c r="D132">
         <v>9.0418353576248318</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>101472507</v>
       </c>
-      <c r="B133">
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
         <v>13.282588011417698</v>
       </c>
-      <c r="C133">
+      <c r="D133">
         <v>8.9214380825565911</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>103996987</v>
       </c>
-      <c r="B134">
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134">
         <v>24.239651575595651</v>
       </c>
-      <c r="C134">
+      <c r="D134">
         <v>24.862238549505243</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>105359284</v>
       </c>
-      <c r="B135">
+      <c r="B135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135">
         <v>13.282588011417698</v>
       </c>
-      <c r="C135">
+      <c r="D135">
         <v>8.0573951434878595</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>106851769</v>
       </c>
-      <c r="B136">
+      <c r="B136" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136">
         <v>2.9440628066732089</v>
       </c>
-      <c r="C136">
+      <c r="D136">
         <v>3.870967741935484</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>107119628</v>
       </c>
-      <c r="B137">
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137">
         <v>20.484175315207136</v>
       </c>
-      <c r="C137">
+      <c r="D137">
         <v>28.829787234042552</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>107367707</v>
       </c>
-      <c r="B138">
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138">
         <v>13.282588011417698</v>
       </c>
-      <c r="C138">
+      <c r="D138">
         <v>8.3715596330275233</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>107553659</v>
       </c>
-      <c r="B139">
+      <c r="B139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139">
         <v>13.285116102017511</v>
       </c>
-      <c r="C139">
+      <c r="D139">
         <v>8.9717741935483879</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>108414390</v>
       </c>
-      <c r="B140">
+      <c r="B140" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140">
         <v>2.6338893766461808</v>
       </c>
-      <c r="C140">
+      <c r="D140">
         <v>3.1446540880503147</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>111302009</v>
       </c>
-      <c r="B141">
+      <c r="B141" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141">
         <v>2.64783759929391</v>
       </c>
-      <c r="C141">
+      <c r="D141">
         <v>3.225806451612903</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>111772276</v>
       </c>
-      <c r="B142">
+      <c r="B142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142">
         <v>13.247049866768176</v>
       </c>
-      <c r="C142">
+      <c r="D142">
         <v>8.1475787855495767</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>112953456</v>
       </c>
-      <c r="B143">
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
         <v>2.64783759929391</v>
       </c>
-      <c r="C143">
+      <c r="D143">
         <v>2.9250457038391224</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>113795698</v>
       </c>
-      <c r="B144">
+      <c r="B144" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144">
         <v>2.64783759929391</v>
       </c>
-      <c r="C144">
+      <c r="D144">
         <v>3.0520646319569122</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>116361990</v>
       </c>
-      <c r="B145">
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145">
         <v>13.332058148431523</v>
       </c>
-      <c r="C145">
+      <c r="D145">
         <v>8.3725305738476017</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>116522779</v>
       </c>
-      <c r="B146">
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146">
         <v>2.64783759929391</v>
       </c>
-      <c r="C146">
+      <c r="D146">
         <v>3.1825795644891124</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>117831469</v>
       </c>
-      <c r="B147">
+      <c r="B147" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147">
         <v>18.901755696675384</v>
       </c>
-      <c r="C147">
+      <c r="D147">
         <v>12.043795620437956</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>117928513</v>
       </c>
-      <c r="B148">
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148">
         <v>2.64783759929391</v>
       </c>
-      <c r="C148">
+      <c r="D148">
         <v>2.5931928687196111</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>118666777</v>
       </c>
-      <c r="B149">
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
         <v>26.73469387755102</v>
       </c>
-      <c r="C149">
+      <c r="D149">
         <v>25.176470588235293</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>119819922</v>
       </c>
-      <c r="B150">
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C150">
+      <c r="D150">
         <v>19.5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>122414437</v>
       </c>
-      <c r="B151">
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151">
         <v>13.939393939393939</v>
       </c>
-      <c r="C151">
+      <c r="D151">
         <v>6.8527918781725887</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>122976077</v>
       </c>
-      <c r="B152">
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152">
         <v>4.0043290043290041</v>
       </c>
-      <c r="C152">
+      <c r="D152">
         <v>2.679658952496955</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>124034426</v>
       </c>
-      <c r="B153">
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153">
         <v>13.939393939393939</v>
       </c>
-      <c r="C153">
+      <c r="D153">
         <v>6.8585944115156643</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>124245472</v>
       </c>
-      <c r="B154">
+      <c r="B154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154">
         <v>13.269780743565301</v>
       </c>
-      <c r="C154">
+      <c r="D154">
         <v>14.496919917864476</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>124260744</v>
       </c>
-      <c r="B155">
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155">
         <v>13.269780743565301</v>
       </c>
-      <c r="C155">
+      <c r="D155">
         <v>14.490968801313629</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>124907477</v>
       </c>
-      <c r="B156">
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156">
         <v>13.333333333333334</v>
       </c>
-      <c r="C156">
+      <c r="D156">
         <v>18.181818181818183</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>126279499</v>
       </c>
-      <c r="B157">
+      <c r="B157" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157">
         <v>23.249299719887954</v>
       </c>
-      <c r="C157">
+      <c r="D157">
         <v>1.5655577299412915</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>126371844</v>
       </c>
-      <c r="B158">
+      <c r="B158" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158">
         <v>13.313046785850133</v>
       </c>
-      <c r="C158">
+      <c r="D158">
         <v>15.548780487804878</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>127966163</v>
       </c>
-      <c r="B159">
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159">
         <v>24.055352584955706</v>
       </c>
-      <c r="C159">
+      <c r="D159">
         <v>31.351069379238393</v>
       </c>
     </row>

</xml_diff>